<commit_message>
VERSION 1.1 YA SE CONECTA
</commit_message>
<xml_diff>
--- a/dispositivos_ejemplo.xlsx
+++ b/dispositivos_ejemplo.xlsx
@@ -1,20 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janet\OneDrive\Documentos\Pragramcion de redes\GIT LEARNING\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{418D6AC2-CB48-41F0-B489-EE56930361C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+  <si>
+    <t>modelo</t>
+  </si>
+  <si>
+    <t>serie</t>
+  </si>
   <si>
     <t>puerto</t>
   </si>
@@ -34,47 +46,32 @@
     <t>dominio</t>
   </si>
   <si>
-    <t>COM3</t>
-  </si>
-  <si>
-    <t>COM4</t>
-  </si>
-  <si>
-    <t>/dev/ttyUSB0</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>Switch1</t>
-  </si>
-  <si>
-    <t>cisco</t>
+    <t>COM8</t>
+  </si>
+  <si>
+    <t>RouterPrueba</t>
   </si>
   <si>
     <t>admin</t>
   </si>
   <si>
-    <t>admin123</t>
-  </si>
-  <si>
-    <t>cisco.com</t>
-  </si>
-  <si>
-    <t>ejemplo.com</t>
-  </si>
-  <si>
-    <t>mi-dominio.local</t>
+    <t>cisco123</t>
+  </si>
+  <si>
+    <t>lab.local</t>
+  </si>
+  <si>
+    <t>CISCO2901/K9</t>
+  </si>
+  <si>
+    <t>FTX153782SQ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,6 +81,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -126,24 +131,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -181,7 +195,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -215,6 +229,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -249,9 +264,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -424,14 +440,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -450,66 +468,41 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2">
         <v>9600</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3">
-        <v>9600</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4">
-        <v>115200</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" t="s">
-        <v>17</v>
-      </c>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H7" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Feat:Se corrgio con ctrl+c y primero leer xcel
</commit_message>
<xml_diff>
--- a/dispositivos_ejemplo.xlsx
+++ b/dispositivos_ejemplo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janet\OneDrive\Documentos\Pragramcion de redes\GIT LEARNING\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{418D6AC2-CB48-41F0-B489-EE56930361C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD1251FB-C6F8-4518-A6A1-E8DD203CDC00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>modelo</t>
   </si>
@@ -46,25 +46,31 @@
     <t>dominio</t>
   </si>
   <si>
-    <t>COM8</t>
-  </si>
-  <si>
-    <t>RouterPrueba</t>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>cisco123</t>
-  </si>
-  <si>
-    <t>lab.local</t>
-  </si>
-  <si>
     <t>CISCO2901/K9</t>
   </si>
   <si>
-    <t>FTX153782SQ</t>
+    <t>cisco</t>
+  </si>
+  <si>
+    <t>FTX144582PJ</t>
+  </si>
+  <si>
+    <t>FTX144583KT</t>
+  </si>
+  <si>
+    <t>R4prueba</t>
+  </si>
+  <si>
+    <t>xime.com</t>
+  </si>
+  <si>
+    <t>unipoli.com</t>
+  </si>
+  <si>
+    <t>COM11</t>
+  </si>
+  <si>
+    <t>nose-FTX144582PJ</t>
   </si>
 </sst>
 </file>
@@ -96,12 +102,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -131,12 +143,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,68 +459,104 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" zoomScale="136" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.5546875" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" customWidth="1"/>
+    <col min="3" max="3" width="13.77734375" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="16.21875" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" customWidth="1"/>
+    <col min="7" max="7" width="17" customWidth="1"/>
+    <col min="8" max="8" width="14.21875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="2">
+        <v>9600</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="2">
+        <v>9600</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2">
-        <v>9600</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H7" s="2"/>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
FEAT: PRUEBA OPTIMIZACION 1 TEXTFSM
</commit_message>
<xml_diff>
--- a/dispositivos_ejemplo.xlsx
+++ b/dispositivos_ejemplo.xlsx
@@ -1,119 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janet\OneDrive\Documentos\Pragramcion de redes\GIT LEARNING\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD1251FB-C6F8-4518-A6A1-E8DD203CDC00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
-  <si>
-    <t>modelo</t>
-  </si>
-  <si>
-    <t>serie</t>
-  </si>
-  <si>
-    <t>puerto</t>
-  </si>
-  <si>
-    <t>baudios</t>
-  </si>
-  <si>
-    <t>nombre</t>
-  </si>
-  <si>
-    <t>usuario</t>
-  </si>
-  <si>
-    <t>contrasena</t>
-  </si>
-  <si>
-    <t>dominio</t>
-  </si>
-  <si>
-    <t>CISCO2901/K9</t>
-  </si>
-  <si>
-    <t>cisco</t>
-  </si>
-  <si>
-    <t>FTX144582PJ</t>
-  </si>
-  <si>
-    <t>FTX144583KT</t>
-  </si>
-  <si>
-    <t>R4prueba</t>
-  </si>
-  <si>
-    <t>xime.com</t>
-  </si>
-  <si>
-    <t>unipoli.com</t>
-  </si>
-  <si>
-    <t>COM11</t>
-  </si>
-  <si>
-    <t>nose-FTX144582PJ</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -125,57 +46,100 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -213,7 +177,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -247,7 +211,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -282,10 +245,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -458,107 +420,142 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="136" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="17.5546875" customWidth="1"/>
-    <col min="2" max="2" width="17.88671875" customWidth="1"/>
-    <col min="3" max="3" width="13.77734375" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" customWidth="1"/>
-    <col min="5" max="5" width="16.21875" customWidth="1"/>
-    <col min="6" max="6" width="15.5546875" customWidth="1"/>
-    <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="14.21875" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>7</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>modelo</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>serie</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>puerto</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>baudios</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>nombre</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>usuario</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>contrasena</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>dominio</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="2">
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>CISCO2901/K9</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>FTX144582PJ</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>COM11</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
         <v>9600</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>13</v>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>nose-FTX144582PJ</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>cisco</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>cisco</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>xime.com</t>
+        </is>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="2">
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>CISCO2901/K9</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>FTX144583KT</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>COM11</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
         <v>9600</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H5" s="1"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>R4prueba</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>cisco</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>cisco</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>unipoli.com</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
FEAT: MODIFY EXPORTACION A EXCEL
</commit_message>
<xml_diff>
--- a/dispositivos_ejemplo.xlsx
+++ b/dispositivos_ejemplo.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,6 +474,11 @@
           <t>dominio</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>interfaces</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -514,6 +519,11 @@
           <t>xime.com</t>
         </is>
       </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>[{'interface': 'GigabitEthernet0/0', 'ip_address': 'unassigned', 'status': 'administratively down', 'proto': 'down'}, {'interface': 'GigabitEthernet0/1', 'ip_address': 'unassigned', 'status': 'administratively down', 'proto': 'down'}, {'interface': 'Serial0/0/0', 'ip_address': 'unassigned', 'status': 'administratively down', 'proto': 'down'}, {'interface': 'Serial0/0/1', 'ip_address': 'unassigned', 'status': 'administratively down', 'proto': 'down'}, {'interface': 'FastEthernet0/2/0', 'ip_address': 'unassigned', 'status': 'administratively down', 'proto': 'down'}, {'interface': 'FastEthernet0/2/1', 'ip_address': 'unassigned', 'status': 'administratively down', 'proto': 'down'}]</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -554,6 +564,7 @@
           <t>unipoli.com</t>
         </is>
       </c>
+      <c r="I3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
FEAT:Optimizacion para las columnas de las interfaces
</commit_message>
<xml_diff>
--- a/dispositivos_ejemplo.xlsx
+++ b/dispositivos_ejemplo.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,62 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>interfaces</t>
+          <t>GigabitEthernet0/0_IP</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>GigabitEthernet0/0_STATUS</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>GigabitEthernet0/0_PROTO</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>GigabitEthernet0/1_IP</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>GigabitEthernet0/1_STATUS</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>GigabitEthernet0/1_PROTO</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>FastEthernet0/2/0_IP</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>FastEthernet0/2/0_STATUS</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>FastEthernet0/2/0_PROTO</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>FastEthernet0/2/1_IP</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>FastEthernet0/2/1_STATUS</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>FastEthernet0/2/1_PROTO</t>
         </is>
       </c>
     </row>
@@ -516,12 +571,67 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>xime.com</t>
+          <t>jane.com</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>[{'interface': 'GigabitEthernet0/0', 'ip_address': 'unassigned', 'status': 'administratively down', 'proto': 'down'}, {'interface': 'GigabitEthernet0/1', 'ip_address': 'unassigned', 'status': 'administratively down', 'proto': 'down'}, {'interface': 'Serial0/0/0', 'ip_address': 'unassigned', 'status': 'administratively down', 'proto': 'down'}, {'interface': 'Serial0/0/1', 'ip_address': 'unassigned', 'status': 'administratively down', 'proto': 'down'}, {'interface': 'FastEthernet0/2/0', 'ip_address': 'unassigned', 'status': 'administratively down', 'proto': 'down'}, {'interface': 'FastEthernet0/2/1', 'ip_address': 'unassigned', 'status': 'administratively down', 'proto': 'down'}]</t>
+          <t>192.168.2.1</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>administratively down</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>down</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>unassigned</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>administratively down</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>down</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>unassigned</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>administratively down</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>down</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>unassigned</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>administratively down</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>down</t>
         </is>
       </c>
     </row>
@@ -565,6 +675,17 @@
         </is>
       </c>
       <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="inlineStr"/>
+      <c r="T3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>